<commit_message>
usman new users added
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C768804
</commit_message>
<xml_diff>
--- a/PPIUK-URLs/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-URLs/src/test/resources/CobaltUsers.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="203">
   <si>
     <t>UserName</t>
   </si>
@@ -457,6 +457,174 @@
   </si>
   <si>
     <t>linking.autouser@mailinator.com</t>
+  </si>
+  <si>
+    <t>SearchOpenWebUser1</t>
+  </si>
+  <si>
+    <t>FFHUser1</t>
+  </si>
+  <si>
+    <t>FFHUser2</t>
+  </si>
+  <si>
+    <t>FFHUser3</t>
+  </si>
+  <si>
+    <t>FFHUser4</t>
+  </si>
+  <si>
+    <t>FrontEndUser1</t>
+  </si>
+  <si>
+    <t>FrontEndUser2</t>
+  </si>
+  <si>
+    <t>FrontEndUser3</t>
+  </si>
+  <si>
+    <t>FrontEndUser4</t>
+  </si>
+  <si>
+    <t>FrontEndUser5</t>
+  </si>
+  <si>
+    <t>FrontEndUser6</t>
+  </si>
+  <si>
+    <t>FrontEndUser7</t>
+  </si>
+  <si>
+    <t>FrontEndUser8</t>
+  </si>
+  <si>
+    <t>FrontEndUser9</t>
+  </si>
+  <si>
+    <t>FrontEndUser10</t>
+  </si>
+  <si>
+    <t>UrlUser1</t>
+  </si>
+  <si>
+    <t>UrlUser2</t>
+  </si>
+  <si>
+    <t>UrlUser3</t>
+  </si>
+  <si>
+    <t>LinkingUser1</t>
+  </si>
+  <si>
+    <t>LoginUser1</t>
+  </si>
+  <si>
+    <t>LoginUser2</t>
+  </si>
+  <si>
+    <t>LoginUser3</t>
+  </si>
+  <si>
+    <t>LoginUser4</t>
+  </si>
+  <si>
+    <t>LoginUser5</t>
+  </si>
+  <si>
+    <t>LoginUser6</t>
+  </si>
+  <si>
+    <t>LoginUser7</t>
+  </si>
+  <si>
+    <t>CpetUser1</t>
+  </si>
+  <si>
+    <t>CpetUser2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchOpenWeb@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FFHUser1@mailinator.com </t>
+  </si>
+  <si>
+    <t>FFHUser2@mailinator.com</t>
+  </si>
+  <si>
+    <t>FFHUser3@mailinator.com</t>
+  </si>
+  <si>
+    <t>FFHUser4@mailinator.com</t>
+  </si>
+  <si>
+    <t>FrontEndUser1@mailinator.com</t>
+  </si>
+  <si>
+    <t>FrontEndUser2@mailinator.com</t>
+  </si>
+  <si>
+    <t>FrontEndUser3@mailinator.com</t>
+  </si>
+  <si>
+    <t>FrontEndUser4@mailinator.com</t>
+  </si>
+  <si>
+    <t>FrontEndUser5@mailinator.com</t>
+  </si>
+  <si>
+    <t>FrontEndUser6@mailinator.com</t>
+  </si>
+  <si>
+    <t>FrontEndUser7@mailinator.com</t>
+  </si>
+  <si>
+    <t>FrontEndUser8@mailinator.com</t>
+  </si>
+  <si>
+    <t>FrontEndUser9@mailinator.com</t>
+  </si>
+  <si>
+    <t>FrontEndUser10@mailinator.com</t>
+  </si>
+  <si>
+    <t>UrlUser1@mailinator.com</t>
+  </si>
+  <si>
+    <t>UrlUser2@mailinator.com</t>
+  </si>
+  <si>
+    <t>UrlUser3@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LinkingUser1@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LoginUser1@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LoginUser2@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LoginUser3@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LoginUser4@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LoginUser5@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LoginUser6@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LoginUser7@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CpetUser1@mailinator.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CpetUser2@mailinator.com </t>
   </si>
 </sst>
 </file>
@@ -502,7 +670,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -538,12 +706,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -553,6 +732,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -614,7 +795,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -649,7 +830,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -858,15 +1039,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
@@ -1904,6 +2085,398 @@
       </c>
       <c r="G52" s="5" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>147</v>
+      </c>
+      <c r="B53" t="s">
+        <v>52</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>148</v>
+      </c>
+      <c r="B54" t="s">
+        <v>52</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>149</v>
+      </c>
+      <c r="B55" t="s">
+        <v>52</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>150</v>
+      </c>
+      <c r="B56" t="s">
+        <v>52</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>151</v>
+      </c>
+      <c r="B57" t="s">
+        <v>52</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>152</v>
+      </c>
+      <c r="B58" t="s">
+        <v>52</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>153</v>
+      </c>
+      <c r="B59" t="s">
+        <v>52</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>154</v>
+      </c>
+      <c r="B60" t="s">
+        <v>52</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>155</v>
+      </c>
+      <c r="B61" t="s">
+        <v>52</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>156</v>
+      </c>
+      <c r="B62" t="s">
+        <v>52</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>157</v>
+      </c>
+      <c r="B63" t="s">
+        <v>52</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>158</v>
+      </c>
+      <c r="B64" t="s">
+        <v>52</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>159</v>
+      </c>
+      <c r="B65" t="s">
+        <v>52</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G65" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>160</v>
+      </c>
+      <c r="B66" t="s">
+        <v>52</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>161</v>
+      </c>
+      <c r="B67" t="s">
+        <v>52</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>162</v>
+      </c>
+      <c r="B68" t="s">
+        <v>52</v>
+      </c>
+      <c r="F68" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G68" s="10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>163</v>
+      </c>
+      <c r="B69" t="s">
+        <v>52</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G69" s="10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>164</v>
+      </c>
+      <c r="B70" t="s">
+        <v>52</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G70" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>165</v>
+      </c>
+      <c r="B71" t="s">
+        <v>52</v>
+      </c>
+      <c r="F71" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G71" s="10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>166</v>
+      </c>
+      <c r="B72" t="s">
+        <v>52</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G72" s="10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>167</v>
+      </c>
+      <c r="B73" t="s">
+        <v>52</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G73" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>168</v>
+      </c>
+      <c r="B74" t="s">
+        <v>52</v>
+      </c>
+      <c r="F74" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G74" s="10" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>169</v>
+      </c>
+      <c r="B75" t="s">
+        <v>52</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G75" s="10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>170</v>
+      </c>
+      <c r="B76" t="s">
+        <v>52</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>171</v>
+      </c>
+      <c r="B77" t="s">
+        <v>52</v>
+      </c>
+      <c r="F77" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G77" s="10" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>172</v>
+      </c>
+      <c r="B78" t="s">
+        <v>52</v>
+      </c>
+      <c r="F78" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G78" s="10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>173</v>
+      </c>
+      <c r="B79" t="s">
+        <v>52</v>
+      </c>
+      <c r="F79" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G79" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>174</v>
+      </c>
+      <c r="B80" t="s">
+        <v>52</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G80" s="10" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -1925,9 +2498,37 @@
     <hyperlink ref="G48" r:id="rId15"/>
     <hyperlink ref="G49" r:id="rId16"/>
     <hyperlink ref="G51" r:id="rId17"/>
+    <hyperlink ref="G55" r:id="rId18"/>
+    <hyperlink ref="G54" r:id="rId19"/>
+    <hyperlink ref="G56" r:id="rId20"/>
+    <hyperlink ref="G57" r:id="rId21"/>
+    <hyperlink ref="G58" r:id="rId22"/>
+    <hyperlink ref="G59" r:id="rId23"/>
+    <hyperlink ref="G60" r:id="rId24"/>
+    <hyperlink ref="G61" r:id="rId25"/>
+    <hyperlink ref="G62" r:id="rId26"/>
+    <hyperlink ref="G63" r:id="rId27"/>
+    <hyperlink ref="G64" r:id="rId28"/>
+    <hyperlink ref="G65" r:id="rId29"/>
+    <hyperlink ref="G66" r:id="rId30"/>
+    <hyperlink ref="G67" r:id="rId31"/>
+    <hyperlink ref="G68" r:id="rId32"/>
+    <hyperlink ref="G69" r:id="rId33"/>
+    <hyperlink ref="G53" r:id="rId34"/>
+    <hyperlink ref="G70" r:id="rId35"/>
+    <hyperlink ref="G71" r:id="rId36"/>
+    <hyperlink ref="G72" r:id="rId37"/>
+    <hyperlink ref="G73" r:id="rId38"/>
+    <hyperlink ref="G74" r:id="rId39"/>
+    <hyperlink ref="G75" r:id="rId40"/>
+    <hyperlink ref="G76" r:id="rId41"/>
+    <hyperlink ref="G77" r:id="rId42"/>
+    <hyperlink ref="G78" r:id="rId43"/>
+    <hyperlink ref="G79" r:id="rId44"/>
+    <hyperlink ref="G80" r:id="rId45"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId46"/>
 </worksheet>
 </file>
 

</xml_diff>